<commit_message>
Fix introduction (1.2) and other pending commits.
git-svn-id: file://localhost/tmp/svn2git/svn@4406 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/tg11-dare/data_tg.xlsx
+++ b/papers/tg11-dare/data_tg.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="159" activeTab="1"/>
+    <workbookView xWindow="1340" yWindow="-200" windowWidth="24800" windowHeight="15860" tabRatio="159" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -163,8 +163,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,15 +229,19 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,104 +288,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -389,7 +301,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="8"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -405,107 +317,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -830,14 +650,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="A3:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
@@ -1148,9 +969,11 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1158,14 +981,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
@@ -1787,10 +1611,11 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
adding file tranfer table
git-svn-id: file://localhost/tmp/svn2git/svn@4414 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/tg11-dare/data_tg.xlsx
+++ b/papers/tg11-dare/data_tg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="159" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="159" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>Genome</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>cloud-SI, QB, Ranger</t>
+  </si>
+  <si>
+    <t>Index files</t>
+  </si>
+  <si>
+    <t>Raw Shortreads</t>
+  </si>
+  <si>
+    <t>processed Shortreads</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -309,6 +318,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -446,7 +469,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -507,6 +530,13 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -569,6 +599,13 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1226,14 +1263,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
@@ -1922,6 +1960,101 @@
         <v>158.33000000000001</v>
       </c>
     </row>
+    <row r="47" spans="1:7">
+      <c r="B47" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="7">
+        <v>127</v>
+      </c>
+      <c r="C48" s="7">
+        <v>9</v>
+      </c>
+      <c r="D48" s="7">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="7">
+        <v>1814.29</v>
+      </c>
+      <c r="C49" s="7">
+        <v>128.57</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="7">
+        <v>21166.67</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="7">
+        <v>7105.67</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="7">
+        <v>158.33000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="7">
+        <v>7105</v>
+      </c>
+      <c r="C53" s="7">
+        <v>128</v>
+      </c>
+      <c r="D53" s="7">
+        <v>158.33000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
namd form with borders
git-svn-id: file://localhost/tmp/svn2git/svn@4425 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/tg11-dare/data_tg.xlsx
+++ b/papers/tg11-dare/data_tg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="159"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="159" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ngs" sheetId="2" r:id="rId1"/>
@@ -223,8 +223,8 @@
     <t>TTC(S)</t>
   </si>
   <si>
-    <t xml:space="preserve">151
-</t>
+    <t xml:space="preserve">
+141</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
@@ -2151,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2203,7 +2203,7 @@
         <v>8</v>
       </c>
       <c r="G4">
-        <v>778</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="30">
@@ -2217,10 +2217,10 @@
         <v>8</v>
       </c>
       <c r="E5">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
file transfer speed data
git-svn-id: file://localhost/tmp/svn2git/svn@4818 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/tg11-dare/data_tg.xlsx
+++ b/papers/tg11-dare/data_tg.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18940" tabRatio="159"/>
+    <workbookView xWindow="2800" yWindow="380" windowWidth="25600" windowHeight="15940" tabRatio="263" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ngs" sheetId="2" r:id="rId1"/>
     <sheet name="namd" sheetId="1" r:id="rId2"/>
+    <sheet name="file transfer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
   <si>
     <t>Genome</t>
   </si>
@@ -227,6 +228,9 @@
   </si>
   <si>
     <t>96 MBPS</t>
+  </si>
+  <si>
+    <t>old Speeds</t>
   </si>
 </sst>
 </file>
@@ -353,7 +357,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -363,6 +367,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -546,7 +560,7 @@
     </xf>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -628,6 +642,11 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -711,6 +730,11 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1042,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1615,7 +1639,7 @@
         <v>0.375</v>
       </c>
       <c r="K24" s="11">
-        <v>0.45833333333333331</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="16" thickTop="1">
@@ -1634,6 +1658,9 @@
       <c r="I25">
         <v>113.17</v>
       </c>
+      <c r="K25">
+        <v>112</v>
+      </c>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="8" t="s">
@@ -1648,14 +1675,16 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
-        <v>22.91</v>
+        <v>26.91</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1">
         <v>23</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="8" t="s">
@@ -2263,7 +2292,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2406,4 +2435,97 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" thickBot="1">
+      <c r="C2" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="11">
+        <v>0.6875</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16" thickTop="1">
+      <c r="A3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>113.17</v>
+      </c>
+      <c r="G3">
+        <v>112</v>
+      </c>
+      <c r="I3">
+        <v>110</v>
+      </c>
+      <c r="K3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1">
+        <v>26.91</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>23.6</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>24.3</v>
+      </c>
+      <c r="I4">
+        <v>24.2</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>